<commit_message>
@Update performance test cases
</commit_message>
<xml_diff>
--- a/resources/templatePerformance.xlsx
+++ b/resources/templatePerformance.xlsx
@@ -626,12 +626,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -648,24 +645,6 @@
     <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -674,6 +653,24 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -692,12 +689,6 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1025,13 +1016,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:27" ht="27.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="18" t="s">
+      <c r="A1" s="14" t="s">
         <v>8</v>
       </c>
       <c r="B1" s="15"/>
     </row>
     <row r="2" spans="1:27" ht="27.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="14" t="s">
+      <c r="A2" s="16" t="s">
         <v>9</v>
       </c>
       <c r="B2" s="15"/>
@@ -1068,10 +1059,10 @@
       <c r="AA3" s="13"/>
     </row>
     <row r="4" spans="1:27" s="1" customFormat="1" ht="27.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="3"/>
+      <c r="A4" s="2"/>
     </row>
     <row r="5" spans="1:27" ht="27.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="14" t="s">
+      <c r="A5" s="16" t="s">
         <v>10</v>
       </c>
       <c r="B5" s="15"/>
@@ -1087,10 +1078,10 @@
       <c r="F6" s="15"/>
     </row>
     <row r="7" spans="1:27" s="1" customFormat="1" ht="27.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="3"/>
+      <c r="A7" s="2"/>
     </row>
     <row r="8" spans="1:27" ht="27.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="14" t="s">
+      <c r="A8" s="16" t="s">
         <v>26</v>
       </c>
       <c r="B8" s="15"/>
@@ -1104,70 +1095,70 @@
       <c r="C9" s="13"/>
       <c r="D9" s="13"/>
       <c r="E9" s="13"/>
-      <c r="F9" s="6"/>
-      <c r="G9" s="6"/>
+      <c r="F9" s="5"/>
+      <c r="G9" s="5"/>
     </row>
     <row r="10" spans="1:27" ht="27.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="11" t="s">
+      <c r="A10" s="17" t="s">
         <v>28</v>
       </c>
-      <c r="B10" s="12"/>
-      <c r="C10" s="12"/>
+      <c r="B10" s="18"/>
+      <c r="C10" s="18"/>
     </row>
     <row r="11" spans="1:27" ht="27.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="11" t="s">
+      <c r="A11" s="17" t="s">
         <v>29</v>
       </c>
-      <c r="B11" s="12"/>
-      <c r="C11" s="12"/>
+      <c r="B11" s="18"/>
+      <c r="C11" s="18"/>
     </row>
     <row r="12" spans="1:27" ht="27.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="11" t="s">
+      <c r="A12" s="17" t="s">
         <v>30</v>
       </c>
-      <c r="B12" s="12"/>
-      <c r="C12" s="12"/>
+      <c r="B12" s="18"/>
+      <c r="C12" s="18"/>
     </row>
     <row r="13" spans="1:27" ht="27.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="11" t="s">
+      <c r="A13" s="17" t="s">
         <v>31</v>
       </c>
-      <c r="B13" s="12"/>
-      <c r="C13" s="12"/>
+      <c r="B13" s="18"/>
+      <c r="C13" s="18"/>
     </row>
     <row r="14" spans="1:27" ht="27.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="11" t="s">
+      <c r="A14" s="17" t="s">
         <v>32</v>
       </c>
-      <c r="B14" s="12"/>
-      <c r="C14" s="12"/>
+      <c r="B14" s="18"/>
+      <c r="C14" s="18"/>
     </row>
     <row r="15" spans="1:27" ht="27.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="11" t="s">
+      <c r="A15" s="17" t="s">
         <v>33</v>
       </c>
-      <c r="B15" s="12"/>
-      <c r="C15" s="12"/>
+      <c r="B15" s="18"/>
+      <c r="C15" s="18"/>
     </row>
     <row r="16" spans="1:27" ht="27.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="11" t="s">
+      <c r="A16" s="17" t="s">
         <v>34</v>
       </c>
-      <c r="B16" s="12"/>
-      <c r="C16" s="12"/>
+      <c r="B16" s="18"/>
+      <c r="C16" s="18"/>
     </row>
     <row r="17" spans="1:6" ht="27.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="11" t="s">
+      <c r="A17" s="17" t="s">
         <v>35</v>
       </c>
-      <c r="B17" s="12"/>
-      <c r="C17" s="12"/>
-    </row>
-    <row r="18" spans="1:6" s="6" customFormat="1" ht="27.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="3"/>
+      <c r="B17" s="18"/>
+      <c r="C17" s="18"/>
+    </row>
+    <row r="18" spans="1:6" s="5" customFormat="1" ht="27.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A18" s="2"/>
     </row>
     <row r="19" spans="1:6" ht="23" x14ac:dyDescent="0.3">
-      <c r="A19" s="14" t="s">
+      <c r="A19" s="16" t="s">
         <v>36</v>
       </c>
       <c r="B19" s="15"/>
@@ -1182,21 +1173,21 @@
       <c r="D20" s="15"/>
     </row>
     <row r="21" spans="1:6" ht="21" x14ac:dyDescent="0.2">
-      <c r="A21" s="21" t="s">
+      <c r="A21" s="12" t="s">
         <v>37</v>
       </c>
-      <c r="B21" s="21"/>
-      <c r="C21" s="21"/>
-      <c r="D21" s="6"/>
+      <c r="B21" s="12"/>
+      <c r="C21" s="12"/>
+      <c r="D21" s="5"/>
     </row>
     <row r="22" spans="1:6" ht="21" x14ac:dyDescent="0.2">
-      <c r="A22" s="21" t="s">
+      <c r="A22" s="12" t="s">
         <v>38</v>
       </c>
-      <c r="B22" s="21"/>
-      <c r="C22" s="21"/>
-      <c r="D22" s="21"/>
-      <c r="E22" s="3"/>
+      <c r="B22" s="12"/>
+      <c r="C22" s="12"/>
+      <c r="D22" s="12"/>
+      <c r="E22" s="2"/>
     </row>
     <row r="23" spans="1:6" ht="21" x14ac:dyDescent="0.2">
       <c r="A23" s="13" t="s">
@@ -1208,78 +1199,65 @@
       <c r="E23" s="13"/>
     </row>
     <row r="24" spans="1:6" ht="21" x14ac:dyDescent="0.3">
-      <c r="A24" s="16" t="s">
+      <c r="A24" s="19" t="s">
         <v>41</v>
       </c>
-      <c r="B24" s="17"/>
-      <c r="C24" s="17"/>
-      <c r="D24" s="17"/>
-      <c r="E24" s="17"/>
-      <c r="F24" s="17"/>
+      <c r="B24" s="20"/>
+      <c r="C24" s="20"/>
+      <c r="D24" s="20"/>
+      <c r="E24" s="20"/>
+      <c r="F24" s="20"/>
     </row>
     <row r="25" spans="1:6" ht="21" x14ac:dyDescent="0.3">
-      <c r="A25" s="7" t="s">
+      <c r="A25" s="6" t="s">
         <v>42</v>
       </c>
-      <c r="B25" s="19" t="s">
+      <c r="B25" s="10" t="s">
         <v>40</v>
       </c>
-      <c r="C25" s="19"/>
-      <c r="D25" s="19"/>
-      <c r="E25" s="19"/>
-      <c r="F25" s="19"/>
+      <c r="C25" s="10"/>
+      <c r="D25" s="10"/>
+      <c r="E25" s="10"/>
+      <c r="F25" s="10"/>
     </row>
     <row r="26" spans="1:6" ht="21" x14ac:dyDescent="0.3">
-      <c r="A26" s="7" t="s">
+      <c r="A26" s="6" t="s">
         <v>43</v>
       </c>
-      <c r="B26" s="20" t="s">
+      <c r="B26" s="11" t="s">
         <v>46</v>
       </c>
-      <c r="C26" s="20"/>
-      <c r="D26" s="20"/>
-      <c r="E26" s="20"/>
-      <c r="F26" s="20"/>
+      <c r="C26" s="11"/>
+      <c r="D26" s="11"/>
+      <c r="E26" s="11"/>
+      <c r="F26" s="11"/>
     </row>
     <row r="27" spans="1:6" ht="21" x14ac:dyDescent="0.3">
-      <c r="A27" s="7" t="s">
+      <c r="A27" s="6" t="s">
         <v>44</v>
       </c>
-      <c r="B27" s="19" t="s">
+      <c r="B27" s="10" t="s">
         <v>47</v>
       </c>
-      <c r="C27" s="19"/>
-      <c r="D27" s="19"/>
-      <c r="E27" s="19"/>
-      <c r="F27" s="19"/>
+      <c r="C27" s="10"/>
+      <c r="D27" s="10"/>
+      <c r="E27" s="10"/>
+      <c r="F27" s="10"/>
     </row>
     <row r="28" spans="1:6" ht="21" x14ac:dyDescent="0.3">
-      <c r="A28" s="7" t="s">
+      <c r="A28" s="6" t="s">
         <v>45</v>
       </c>
-      <c r="B28" s="20" t="s">
+      <c r="B28" s="11" t="s">
         <v>48</v>
       </c>
-      <c r="C28" s="20"/>
-      <c r="D28" s="20"/>
-      <c r="E28" s="20"/>
-      <c r="F28" s="20"/>
+      <c r="C28" s="11"/>
+      <c r="D28" s="11"/>
+      <c r="E28" s="11"/>
+      <c r="F28" s="11"/>
     </row>
   </sheetData>
   <mergeCells count="25">
-    <mergeCell ref="B25:F25"/>
-    <mergeCell ref="B26:F26"/>
-    <mergeCell ref="B27:F27"/>
-    <mergeCell ref="B28:F28"/>
-    <mergeCell ref="A21:C21"/>
-    <mergeCell ref="A22:D22"/>
-    <mergeCell ref="A23:E23"/>
-    <mergeCell ref="A1:B1"/>
-    <mergeCell ref="A5:B5"/>
-    <mergeCell ref="A8:C8"/>
-    <mergeCell ref="A6:F6"/>
-    <mergeCell ref="A3:AA3"/>
-    <mergeCell ref="A2:B2"/>
     <mergeCell ref="A12:C12"/>
     <mergeCell ref="A9:E9"/>
     <mergeCell ref="A19:C19"/>
@@ -1292,6 +1270,19 @@
     <mergeCell ref="A17:C17"/>
     <mergeCell ref="A10:C10"/>
     <mergeCell ref="A11:C11"/>
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="A5:B5"/>
+    <mergeCell ref="A8:C8"/>
+    <mergeCell ref="A6:F6"/>
+    <mergeCell ref="A3:AA3"/>
+    <mergeCell ref="A2:B2"/>
+    <mergeCell ref="B25:F25"/>
+    <mergeCell ref="B26:F26"/>
+    <mergeCell ref="B27:F27"/>
+    <mergeCell ref="B28:F28"/>
+    <mergeCell ref="A21:C21"/>
+    <mergeCell ref="A22:D22"/>
+    <mergeCell ref="A23:E23"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1315,46 +1306,46 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="27" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="16" t="s">
+      <c r="A1" s="19" t="s">
         <v>87</v>
       </c>
-      <c r="B1" s="16"/>
+      <c r="B1" s="19"/>
     </row>
     <row r="2" spans="1:2" ht="27" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="9" t="s">
+      <c r="A2" s="8" t="s">
         <v>86</v>
       </c>
-      <c r="B2" s="8"/>
+      <c r="B2" s="7"/>
     </row>
     <row r="3" spans="1:2" ht="27" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="7" t="s">
+      <c r="A3" s="6" t="s">
         <v>84</v>
       </c>
-      <c r="B3" s="8"/>
+      <c r="B3" s="7"/>
     </row>
     <row r="4" spans="1:2" ht="27" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="7" t="s">
+      <c r="A4" s="6" t="s">
         <v>79</v>
       </c>
-      <c r="B4" s="8"/>
+      <c r="B4" s="7"/>
     </row>
     <row r="5" spans="1:2" ht="27" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="7" t="s">
+      <c r="A5" s="6" t="s">
         <v>80</v>
       </c>
-      <c r="B5" s="8"/>
+      <c r="B5" s="7"/>
     </row>
     <row r="6" spans="1:2" ht="27" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="7" t="s">
+      <c r="A6" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="B6" s="8"/>
+      <c r="B6" s="7"/>
     </row>
     <row r="7" spans="1:2" ht="27" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="7" t="s">
+      <c r="A7" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="B7" s="8"/>
+      <c r="B7" s="7"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -1380,116 +1371,123 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="27.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="22" t="s">
+      <c r="A1" s="21" t="s">
         <v>11</v>
       </c>
-      <c r="B1" s="23"/>
+      <c r="B1" s="22"/>
     </row>
     <row r="2" spans="1:5" ht="27.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="25" t="s">
+      <c r="A2" s="24" t="s">
         <v>12</v>
       </c>
-      <c r="B2" s="25"/>
+      <c r="B2" s="24"/>
     </row>
     <row r="3" spans="1:5" ht="27.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="17" t="s">
+      <c r="A3" s="20" t="s">
         <v>6</v>
       </c>
-      <c r="B3" s="16"/>
-      <c r="C3" s="16"/>
-      <c r="D3" s="16"/>
-      <c r="E3" s="2"/>
+      <c r="B3" s="20"/>
+      <c r="C3" s="20"/>
+      <c r="D3" s="20"/>
+      <c r="E3" s="20"/>
     </row>
     <row r="4" spans="1:5" ht="27.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="16" t="s">
+      <c r="A4" s="19" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="16"/>
-      <c r="C4" s="29"/>
-      <c r="D4" s="29"/>
+      <c r="B4" s="19"/>
+      <c r="C4" s="26"/>
+      <c r="D4" s="26"/>
+      <c r="E4" s="26"/>
     </row>
     <row r="5" spans="1:5" ht="27.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="16" t="s">
+      <c r="A5" s="19" t="s">
         <v>7</v>
       </c>
-      <c r="B5" s="16"/>
-      <c r="C5" s="29"/>
-      <c r="D5" s="29"/>
-    </row>
-    <row r="6" spans="1:5" s="5" customFormat="1" ht="27.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="4"/>
+      <c r="B5" s="19"/>
+      <c r="C5" s="26"/>
+      <c r="D5" s="26"/>
+      <c r="E5" s="26"/>
+    </row>
+    <row r="6" spans="1:5" s="4" customFormat="1" ht="27.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="3"/>
     </row>
     <row r="7" spans="1:5" ht="27.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="25" t="s">
+      <c r="A7" s="24" t="s">
         <v>13</v>
       </c>
-      <c r="B7" s="25"/>
+      <c r="B7" s="24"/>
     </row>
     <row r="8" spans="1:5" ht="27.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="17" t="s">
+      <c r="A8" s="20" t="s">
         <v>3</v>
       </c>
-      <c r="B8" s="16"/>
-      <c r="C8" s="16"/>
-      <c r="D8" s="16"/>
+      <c r="B8" s="20"/>
+      <c r="C8" s="20"/>
+      <c r="D8" s="20"/>
+      <c r="E8" s="20"/>
     </row>
     <row r="9" spans="1:5" ht="27.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="17" t="s">
+      <c r="A9" s="20" t="s">
         <v>4</v>
       </c>
-      <c r="B9" s="16"/>
-      <c r="C9" s="28"/>
-      <c r="D9" s="28"/>
+      <c r="B9" s="19"/>
+      <c r="C9" s="10"/>
+      <c r="D9" s="10"/>
+      <c r="E9" s="10"/>
     </row>
     <row r="10" spans="1:5" ht="27.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="16" t="s">
+      <c r="A10" s="19" t="s">
         <v>49</v>
       </c>
-      <c r="B10" s="16"/>
-      <c r="C10" s="28"/>
-      <c r="D10" s="28"/>
-    </row>
-    <row r="11" spans="1:5" s="5" customFormat="1" ht="27.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="4"/>
+      <c r="B10" s="19"/>
+      <c r="C10" s="10"/>
+      <c r="D10" s="10"/>
+      <c r="E10" s="10"/>
+    </row>
+    <row r="11" spans="1:5" s="4" customFormat="1" ht="27.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="3"/>
     </row>
     <row r="12" spans="1:5" ht="27.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="24" t="s">
+      <c r="A12" s="23" t="s">
         <v>14</v>
       </c>
-      <c r="B12" s="25"/>
+      <c r="B12" s="24"/>
     </row>
     <row r="13" spans="1:5" ht="27.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="17" t="s">
+      <c r="A13" s="20" t="s">
         <v>5</v>
       </c>
-      <c r="B13" s="16"/>
-      <c r="C13" s="16"/>
-      <c r="D13" s="16"/>
+      <c r="B13" s="20"/>
+      <c r="C13" s="20"/>
+      <c r="D13" s="20"/>
+      <c r="E13" s="20"/>
     </row>
     <row r="14" spans="1:5" ht="27.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="26"/>
-      <c r="B14" s="27"/>
-      <c r="C14" s="27"/>
-      <c r="D14" s="27"/>
+      <c r="A14" s="25"/>
+      <c r="B14" s="25"/>
+      <c r="C14" s="25"/>
+      <c r="D14" s="25"/>
+      <c r="E14" s="25"/>
     </row>
   </sheetData>
   <mergeCells count="16">
+    <mergeCell ref="A13:E13"/>
+    <mergeCell ref="A8:E8"/>
+    <mergeCell ref="A14:E14"/>
+    <mergeCell ref="A3:E3"/>
+    <mergeCell ref="C4:E4"/>
+    <mergeCell ref="C9:E9"/>
+    <mergeCell ref="C10:E10"/>
+    <mergeCell ref="C5:E5"/>
     <mergeCell ref="A1:B1"/>
     <mergeCell ref="A12:B12"/>
-    <mergeCell ref="A13:D13"/>
-    <mergeCell ref="A14:D14"/>
     <mergeCell ref="A9:B9"/>
-    <mergeCell ref="C9:D9"/>
     <mergeCell ref="A7:B7"/>
     <mergeCell ref="A2:B2"/>
     <mergeCell ref="A4:B4"/>
     <mergeCell ref="A5:B5"/>
-    <mergeCell ref="C4:D4"/>
-    <mergeCell ref="C5:D5"/>
-    <mergeCell ref="A3:D3"/>
-    <mergeCell ref="A8:D8"/>
     <mergeCell ref="A10:B10"/>
-    <mergeCell ref="C10:D10"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1514,106 +1512,106 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="27.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="16" t="s">
+      <c r="A1" s="19" t="s">
         <v>50</v>
       </c>
-      <c r="B1" s="16"/>
-      <c r="C1" s="16"/>
-      <c r="D1" s="16"/>
-      <c r="E1" s="16"/>
-      <c r="F1" s="16"/>
-      <c r="G1" s="16"/>
-      <c r="H1" s="16"/>
-      <c r="I1" s="16"/>
-      <c r="J1" s="16"/>
+      <c r="B1" s="19"/>
+      <c r="C1" s="19"/>
+      <c r="D1" s="19"/>
+      <c r="E1" s="19"/>
+      <c r="F1" s="19"/>
+      <c r="G1" s="19"/>
+      <c r="H1" s="19"/>
+      <c r="I1" s="19"/>
+      <c r="J1" s="19"/>
     </row>
     <row r="2" spans="1:10" ht="27.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="7" t="s">
+      <c r="A2" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="B2" s="9" t="s">
+      <c r="B2" s="8" t="s">
         <v>52</v>
       </c>
-      <c r="C2" s="7" t="s">
+      <c r="C2" s="6" t="s">
         <v>53</v>
       </c>
-      <c r="D2" s="7" t="s">
+      <c r="D2" s="6" t="s">
         <v>54</v>
       </c>
-      <c r="E2" s="7" t="s">
+      <c r="E2" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="F2" s="7" t="s">
+      <c r="F2" s="6" t="s">
         <v>55</v>
       </c>
-      <c r="G2" s="7" t="s">
+      <c r="G2" s="6" t="s">
         <v>56</v>
       </c>
-      <c r="H2" s="7" t="s">
+      <c r="H2" s="6" t="s">
         <v>57</v>
       </c>
-      <c r="I2" s="7" t="s">
+      <c r="I2" s="6" t="s">
         <v>58</v>
       </c>
-      <c r="J2" s="7" t="s">
+      <c r="J2" s="6" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="3" spans="1:10" ht="27.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="7" t="s">
+      <c r="A3" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="B3" s="8"/>
-      <c r="C3" s="8"/>
-      <c r="D3" s="8"/>
-      <c r="E3" s="8"/>
-      <c r="F3" s="8"/>
-      <c r="G3" s="8"/>
-      <c r="H3" s="8"/>
-      <c r="I3" s="8"/>
-      <c r="J3" s="8"/>
+      <c r="B3" s="7"/>
+      <c r="C3" s="7"/>
+      <c r="D3" s="7"/>
+      <c r="E3" s="7"/>
+      <c r="F3" s="7"/>
+      <c r="G3" s="7"/>
+      <c r="H3" s="7"/>
+      <c r="I3" s="7"/>
+      <c r="J3" s="7"/>
     </row>
     <row r="4" spans="1:10" ht="27.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="7" t="s">
+      <c r="A4" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="B4" s="10"/>
-      <c r="C4" s="10"/>
-      <c r="D4" s="10"/>
-      <c r="E4" s="10"/>
-      <c r="F4" s="10"/>
-      <c r="G4" s="10"/>
-      <c r="H4" s="10"/>
-      <c r="I4" s="10"/>
-      <c r="J4" s="10"/>
+      <c r="B4" s="9"/>
+      <c r="C4" s="9"/>
+      <c r="D4" s="9"/>
+      <c r="E4" s="9"/>
+      <c r="F4" s="9"/>
+      <c r="G4" s="9"/>
+      <c r="H4" s="9"/>
+      <c r="I4" s="9"/>
+      <c r="J4" s="9"/>
     </row>
     <row r="5" spans="1:10" ht="27.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="7" t="s">
+      <c r="A5" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="B5" s="8"/>
-      <c r="C5" s="8"/>
-      <c r="D5" s="8"/>
-      <c r="E5" s="8"/>
-      <c r="F5" s="8"/>
-      <c r="G5" s="8"/>
-      <c r="H5" s="8"/>
-      <c r="I5" s="8"/>
-      <c r="J5" s="8"/>
+      <c r="B5" s="7"/>
+      <c r="C5" s="7"/>
+      <c r="D5" s="7"/>
+      <c r="E5" s="7"/>
+      <c r="F5" s="7"/>
+      <c r="G5" s="7"/>
+      <c r="H5" s="7"/>
+      <c r="I5" s="7"/>
+      <c r="J5" s="7"/>
     </row>
     <row r="6" spans="1:10" ht="27.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="7" t="s">
+      <c r="A6" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="B6" s="10"/>
-      <c r="C6" s="10"/>
-      <c r="D6" s="10"/>
-      <c r="E6" s="10"/>
-      <c r="F6" s="10"/>
-      <c r="G6" s="10"/>
-      <c r="H6" s="10"/>
-      <c r="I6" s="10"/>
-      <c r="J6" s="10"/>
+      <c r="B6" s="9"/>
+      <c r="C6" s="9"/>
+      <c r="D6" s="9"/>
+      <c r="E6" s="9"/>
+      <c r="F6" s="9"/>
+      <c r="G6" s="9"/>
+      <c r="H6" s="9"/>
+      <c r="I6" s="9"/>
+      <c r="J6" s="9"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -1644,98 +1642,98 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="27.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="16" t="s">
+      <c r="A1" s="19" t="s">
         <v>51</v>
       </c>
-      <c r="B1" s="16"/>
-      <c r="C1" s="16"/>
-      <c r="D1" s="16"/>
-      <c r="E1" s="16"/>
-      <c r="F1" s="16"/>
-      <c r="G1" s="16"/>
-      <c r="H1" s="16"/>
-      <c r="I1" s="16"/>
+      <c r="B1" s="19"/>
+      <c r="C1" s="19"/>
+      <c r="D1" s="19"/>
+      <c r="E1" s="19"/>
+      <c r="F1" s="19"/>
+      <c r="G1" s="19"/>
+      <c r="H1" s="19"/>
+      <c r="I1" s="19"/>
     </row>
     <row r="2" spans="1:9" ht="27.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="7" t="s">
+      <c r="A2" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="B2" s="9" t="s">
+      <c r="B2" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="C2" s="7" t="s">
+      <c r="C2" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="D2" s="7" t="s">
+      <c r="D2" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="E2" s="7" t="s">
+      <c r="E2" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="F2" s="7" t="s">
+      <c r="F2" s="6" t="s">
         <v>59</v>
       </c>
-      <c r="G2" s="7" t="s">
+      <c r="G2" s="6" t="s">
         <v>60</v>
       </c>
-      <c r="H2" s="7" t="s">
+      <c r="H2" s="6" t="s">
         <v>61</v>
       </c>
-      <c r="I2" s="7" t="s">
+      <c r="I2" s="6" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="3" spans="1:9" ht="27.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="7" t="s">
+      <c r="A3" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="B3" s="8"/>
-      <c r="C3" s="8"/>
-      <c r="D3" s="8"/>
-      <c r="E3" s="8"/>
-      <c r="F3" s="8"/>
-      <c r="G3" s="8"/>
-      <c r="H3" s="8"/>
-      <c r="I3" s="8"/>
+      <c r="B3" s="7"/>
+      <c r="C3" s="7"/>
+      <c r="D3" s="7"/>
+      <c r="E3" s="7"/>
+      <c r="F3" s="7"/>
+      <c r="G3" s="7"/>
+      <c r="H3" s="7"/>
+      <c r="I3" s="7"/>
     </row>
     <row r="4" spans="1:9" ht="27.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="7" t="s">
+      <c r="A4" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="B4" s="10"/>
-      <c r="C4" s="10"/>
-      <c r="D4" s="10"/>
-      <c r="E4" s="10"/>
-      <c r="F4" s="10"/>
-      <c r="G4" s="10"/>
-      <c r="H4" s="10"/>
-      <c r="I4" s="10"/>
+      <c r="B4" s="9"/>
+      <c r="C4" s="9"/>
+      <c r="D4" s="9"/>
+      <c r="E4" s="9"/>
+      <c r="F4" s="9"/>
+      <c r="G4" s="9"/>
+      <c r="H4" s="9"/>
+      <c r="I4" s="9"/>
     </row>
     <row r="5" spans="1:9" ht="27.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="7" t="s">
+      <c r="A5" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="B5" s="8"/>
-      <c r="C5" s="8"/>
-      <c r="D5" s="8"/>
-      <c r="E5" s="8"/>
-      <c r="F5" s="8"/>
-      <c r="G5" s="8"/>
-      <c r="H5" s="8"/>
-      <c r="I5" s="8"/>
+      <c r="B5" s="7"/>
+      <c r="C5" s="7"/>
+      <c r="D5" s="7"/>
+      <c r="E5" s="7"/>
+      <c r="F5" s="7"/>
+      <c r="G5" s="7"/>
+      <c r="H5" s="7"/>
+      <c r="I5" s="7"/>
     </row>
     <row r="6" spans="1:9" ht="27.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="7" t="s">
+      <c r="A6" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="B6" s="10"/>
-      <c r="C6" s="10"/>
-      <c r="D6" s="10"/>
-      <c r="E6" s="10"/>
-      <c r="F6" s="10"/>
-      <c r="G6" s="10"/>
-      <c r="H6" s="10"/>
-      <c r="I6" s="10"/>
+      <c r="B6" s="9"/>
+      <c r="C6" s="9"/>
+      <c r="D6" s="9"/>
+      <c r="E6" s="9"/>
+      <c r="F6" s="9"/>
+      <c r="G6" s="9"/>
+      <c r="H6" s="9"/>
+      <c r="I6" s="9"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -1766,122 +1764,122 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="27.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="16" t="s">
+      <c r="A1" s="19" t="s">
         <v>71</v>
       </c>
-      <c r="B1" s="16"/>
-      <c r="C1" s="16"/>
-      <c r="D1" s="16"/>
-      <c r="E1" s="16"/>
-      <c r="F1" s="16"/>
-      <c r="G1" s="16"/>
-      <c r="H1" s="16"/>
-      <c r="I1" s="16"/>
-      <c r="J1" s="16"/>
-      <c r="K1" s="16"/>
-      <c r="L1" s="16"/>
+      <c r="B1" s="19"/>
+      <c r="C1" s="19"/>
+      <c r="D1" s="19"/>
+      <c r="E1" s="19"/>
+      <c r="F1" s="19"/>
+      <c r="G1" s="19"/>
+      <c r="H1" s="19"/>
+      <c r="I1" s="19"/>
+      <c r="J1" s="19"/>
+      <c r="K1" s="19"/>
+      <c r="L1" s="19"/>
     </row>
     <row r="2" spans="1:12" ht="27.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="7" t="s">
+      <c r="A2" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="B2" s="9" t="s">
+      <c r="B2" s="8" t="s">
         <v>62</v>
       </c>
-      <c r="C2" s="7" t="s">
+      <c r="C2" s="6" t="s">
         <v>63</v>
       </c>
-      <c r="D2" s="7" t="s">
+      <c r="D2" s="6" t="s">
         <v>64</v>
       </c>
-      <c r="E2" s="7" t="s">
+      <c r="E2" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="F2" s="7" t="s">
+      <c r="F2" s="6" t="s">
         <v>65</v>
       </c>
-      <c r="G2" s="7" t="s">
+      <c r="G2" s="6" t="s">
         <v>66</v>
       </c>
-      <c r="H2" s="7" t="s">
+      <c r="H2" s="6" t="s">
         <v>67</v>
       </c>
-      <c r="I2" s="7" t="s">
+      <c r="I2" s="6" t="s">
         <v>68</v>
       </c>
-      <c r="J2" s="7" t="s">
+      <c r="J2" s="6" t="s">
         <v>69</v>
       </c>
-      <c r="K2" s="7" t="s">
+      <c r="K2" s="6" t="s">
         <v>70</v>
       </c>
-      <c r="L2" s="7" t="s">
+      <c r="L2" s="6" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="3" spans="1:12" ht="27.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="7" t="s">
+      <c r="A3" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="B3" s="8"/>
-      <c r="C3" s="8"/>
-      <c r="D3" s="8"/>
-      <c r="E3" s="8"/>
-      <c r="F3" s="8"/>
-      <c r="G3" s="8"/>
-      <c r="H3" s="8"/>
-      <c r="I3" s="8"/>
-      <c r="J3" s="8"/>
-      <c r="K3" s="8"/>
-      <c r="L3" s="8"/>
+      <c r="B3" s="7"/>
+      <c r="C3" s="7"/>
+      <c r="D3" s="7"/>
+      <c r="E3" s="7"/>
+      <c r="F3" s="7"/>
+      <c r="G3" s="7"/>
+      <c r="H3" s="7"/>
+      <c r="I3" s="7"/>
+      <c r="J3" s="7"/>
+      <c r="K3" s="7"/>
+      <c r="L3" s="7"/>
     </row>
     <row r="4" spans="1:12" ht="27.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="7" t="s">
+      <c r="A4" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="B4" s="10"/>
-      <c r="C4" s="10"/>
-      <c r="D4" s="10"/>
-      <c r="E4" s="10"/>
-      <c r="F4" s="10"/>
-      <c r="G4" s="10"/>
-      <c r="H4" s="10"/>
-      <c r="I4" s="10"/>
-      <c r="J4" s="10"/>
-      <c r="K4" s="10"/>
-      <c r="L4" s="10"/>
+      <c r="B4" s="9"/>
+      <c r="C4" s="9"/>
+      <c r="D4" s="9"/>
+      <c r="E4" s="9"/>
+      <c r="F4" s="9"/>
+      <c r="G4" s="9"/>
+      <c r="H4" s="9"/>
+      <c r="I4" s="9"/>
+      <c r="J4" s="9"/>
+      <c r="K4" s="9"/>
+      <c r="L4" s="9"/>
     </row>
     <row r="5" spans="1:12" ht="27.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="7" t="s">
+      <c r="A5" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="B5" s="8"/>
-      <c r="C5" s="8"/>
-      <c r="D5" s="8"/>
-      <c r="E5" s="8"/>
-      <c r="F5" s="8"/>
-      <c r="G5" s="8"/>
-      <c r="H5" s="8"/>
-      <c r="I5" s="8"/>
-      <c r="J5" s="8"/>
-      <c r="K5" s="8"/>
-      <c r="L5" s="8"/>
+      <c r="B5" s="7"/>
+      <c r="C5" s="7"/>
+      <c r="D5" s="7"/>
+      <c r="E5" s="7"/>
+      <c r="F5" s="7"/>
+      <c r="G5" s="7"/>
+      <c r="H5" s="7"/>
+      <c r="I5" s="7"/>
+      <c r="J5" s="7"/>
+      <c r="K5" s="7"/>
+      <c r="L5" s="7"/>
     </row>
     <row r="6" spans="1:12" ht="27.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="7" t="s">
+      <c r="A6" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="B6" s="10"/>
-      <c r="C6" s="10"/>
-      <c r="D6" s="10"/>
-      <c r="E6" s="10"/>
-      <c r="F6" s="10"/>
-      <c r="G6" s="10"/>
-      <c r="H6" s="10"/>
-      <c r="I6" s="10"/>
-      <c r="J6" s="10"/>
-      <c r="K6" s="10"/>
-      <c r="L6" s="10"/>
+      <c r="B6" s="9"/>
+      <c r="C6" s="9"/>
+      <c r="D6" s="9"/>
+      <c r="E6" s="9"/>
+      <c r="F6" s="9"/>
+      <c r="G6" s="9"/>
+      <c r="H6" s="9"/>
+      <c r="I6" s="9"/>
+      <c r="J6" s="9"/>
+      <c r="K6" s="9"/>
+      <c r="L6" s="9"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -1911,114 +1909,114 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="27.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="16" t="s">
+      <c r="A1" s="19" t="s">
         <v>72</v>
       </c>
-      <c r="B1" s="16"/>
-      <c r="C1" s="16"/>
-      <c r="D1" s="16"/>
-      <c r="E1" s="16"/>
-      <c r="F1" s="16"/>
-      <c r="G1" s="16"/>
-      <c r="H1" s="16"/>
-      <c r="I1" s="16"/>
-      <c r="J1" s="16"/>
-      <c r="K1" s="16"/>
+      <c r="B1" s="19"/>
+      <c r="C1" s="19"/>
+      <c r="D1" s="19"/>
+      <c r="E1" s="19"/>
+      <c r="F1" s="19"/>
+      <c r="G1" s="19"/>
+      <c r="H1" s="19"/>
+      <c r="I1" s="19"/>
+      <c r="J1" s="19"/>
+      <c r="K1" s="19"/>
     </row>
     <row r="2" spans="1:11" ht="27.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="7" t="s">
+      <c r="A2" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="B2" s="9" t="s">
+      <c r="B2" s="8" t="s">
         <v>62</v>
       </c>
-      <c r="C2" s="7" t="s">
+      <c r="C2" s="6" t="s">
         <v>63</v>
       </c>
-      <c r="D2" s="7" t="s">
+      <c r="D2" s="6" t="s">
         <v>64</v>
       </c>
-      <c r="E2" s="7" t="s">
+      <c r="E2" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="F2" s="7" t="s">
+      <c r="F2" s="6" t="s">
         <v>66</v>
       </c>
-      <c r="G2" s="7" t="s">
+      <c r="G2" s="6" t="s">
         <v>67</v>
       </c>
-      <c r="H2" s="7" t="s">
+      <c r="H2" s="6" t="s">
         <v>68</v>
       </c>
-      <c r="I2" s="7" t="s">
+      <c r="I2" s="6" t="s">
         <v>69</v>
       </c>
-      <c r="J2" s="7" t="s">
+      <c r="J2" s="6" t="s">
         <v>70</v>
       </c>
-      <c r="K2" s="7" t="s">
+      <c r="K2" s="6" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="3" spans="1:11" ht="27.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="7" t="s">
+      <c r="A3" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="B3" s="8"/>
-      <c r="C3" s="8"/>
-      <c r="D3" s="8"/>
-      <c r="E3" s="8"/>
-      <c r="F3" s="8"/>
-      <c r="G3" s="8"/>
-      <c r="H3" s="8"/>
-      <c r="I3" s="8"/>
-      <c r="J3" s="8"/>
-      <c r="K3" s="8"/>
+      <c r="B3" s="7"/>
+      <c r="C3" s="7"/>
+      <c r="D3" s="7"/>
+      <c r="E3" s="7"/>
+      <c r="F3" s="7"/>
+      <c r="G3" s="7"/>
+      <c r="H3" s="7"/>
+      <c r="I3" s="7"/>
+      <c r="J3" s="7"/>
+      <c r="K3" s="7"/>
     </row>
     <row r="4" spans="1:11" ht="27.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="7" t="s">
+      <c r="A4" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="B4" s="10"/>
-      <c r="C4" s="10"/>
-      <c r="D4" s="10"/>
-      <c r="E4" s="10"/>
-      <c r="F4" s="10"/>
-      <c r="G4" s="10"/>
-      <c r="H4" s="10"/>
-      <c r="I4" s="10"/>
-      <c r="J4" s="10"/>
-      <c r="K4" s="10"/>
+      <c r="B4" s="9"/>
+      <c r="C4" s="9"/>
+      <c r="D4" s="9"/>
+      <c r="E4" s="9"/>
+      <c r="F4" s="9"/>
+      <c r="G4" s="9"/>
+      <c r="H4" s="9"/>
+      <c r="I4" s="9"/>
+      <c r="J4" s="9"/>
+      <c r="K4" s="9"/>
     </row>
     <row r="5" spans="1:11" ht="27.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="7" t="s">
+      <c r="A5" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="B5" s="8"/>
-      <c r="C5" s="8"/>
-      <c r="D5" s="8"/>
-      <c r="E5" s="8"/>
-      <c r="F5" s="8"/>
-      <c r="G5" s="8"/>
-      <c r="H5" s="8"/>
-      <c r="I5" s="8"/>
-      <c r="J5" s="8"/>
-      <c r="K5" s="8"/>
+      <c r="B5" s="7"/>
+      <c r="C5" s="7"/>
+      <c r="D5" s="7"/>
+      <c r="E5" s="7"/>
+      <c r="F5" s="7"/>
+      <c r="G5" s="7"/>
+      <c r="H5" s="7"/>
+      <c r="I5" s="7"/>
+      <c r="J5" s="7"/>
+      <c r="K5" s="7"/>
     </row>
     <row r="6" spans="1:11" ht="27.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="7" t="s">
+      <c r="A6" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="B6" s="10"/>
-      <c r="C6" s="10"/>
-      <c r="D6" s="10"/>
-      <c r="E6" s="10"/>
-      <c r="F6" s="10"/>
-      <c r="G6" s="10"/>
-      <c r="H6" s="10"/>
-      <c r="I6" s="10"/>
-      <c r="J6" s="10"/>
-      <c r="K6" s="10"/>
+      <c r="B6" s="9"/>
+      <c r="C6" s="9"/>
+      <c r="D6" s="9"/>
+      <c r="E6" s="9"/>
+      <c r="F6" s="9"/>
+      <c r="G6" s="9"/>
+      <c r="H6" s="9"/>
+      <c r="I6" s="9"/>
+      <c r="J6" s="9"/>
+      <c r="K6" s="9"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -2047,90 +2045,90 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="27" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="16" t="s">
+      <c r="A1" s="19" t="s">
         <v>73</v>
       </c>
-      <c r="B1" s="16"/>
-      <c r="C1" s="16"/>
-      <c r="D1" s="16"/>
-      <c r="E1" s="16"/>
-      <c r="F1" s="16"/>
-      <c r="G1" s="16"/>
-      <c r="H1" s="16"/>
+      <c r="B1" s="19"/>
+      <c r="C1" s="19"/>
+      <c r="D1" s="19"/>
+      <c r="E1" s="19"/>
+      <c r="F1" s="19"/>
+      <c r="G1" s="19"/>
+      <c r="H1" s="19"/>
     </row>
     <row r="2" spans="1:8" ht="27" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="7" t="s">
+      <c r="A2" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="B2" s="9" t="s">
+      <c r="B2" s="8" t="s">
         <v>74</v>
       </c>
-      <c r="C2" s="7" t="s">
+      <c r="C2" s="6" t="s">
         <v>75</v>
       </c>
-      <c r="D2" s="7" t="s">
+      <c r="D2" s="6" t="s">
         <v>76</v>
       </c>
-      <c r="E2" s="7" t="s">
+      <c r="E2" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="F2" s="7" t="s">
+      <c r="F2" s="6" t="s">
         <v>77</v>
       </c>
-      <c r="G2" s="7" t="s">
+      <c r="G2" s="6" t="s">
         <v>78</v>
       </c>
-      <c r="H2" s="7" t="s">
+      <c r="H2" s="6" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="3" spans="1:8" ht="27" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="7" t="s">
+      <c r="A3" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="B3" s="8"/>
-      <c r="C3" s="8"/>
-      <c r="D3" s="8"/>
-      <c r="E3" s="8"/>
-      <c r="F3" s="8"/>
-      <c r="G3" s="8"/>
-      <c r="H3" s="8"/>
+      <c r="B3" s="7"/>
+      <c r="C3" s="7"/>
+      <c r="D3" s="7"/>
+      <c r="E3" s="7"/>
+      <c r="F3" s="7"/>
+      <c r="G3" s="7"/>
+      <c r="H3" s="7"/>
     </row>
     <row r="4" spans="1:8" ht="27" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="7" t="s">
+      <c r="A4" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="B4" s="10"/>
-      <c r="C4" s="10"/>
-      <c r="D4" s="10"/>
-      <c r="E4" s="10"/>
-      <c r="F4" s="10"/>
-      <c r="G4" s="10"/>
-      <c r="H4" s="10"/>
+      <c r="B4" s="9"/>
+      <c r="C4" s="9"/>
+      <c r="D4" s="9"/>
+      <c r="E4" s="9"/>
+      <c r="F4" s="9"/>
+      <c r="G4" s="9"/>
+      <c r="H4" s="9"/>
     </row>
     <row r="5" spans="1:8" ht="27" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="7" t="s">
+      <c r="A5" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="B5" s="8"/>
-      <c r="C5" s="8"/>
-      <c r="D5" s="8"/>
-      <c r="E5" s="8"/>
-      <c r="F5" s="8"/>
-      <c r="G5" s="8"/>
-      <c r="H5" s="8"/>
+      <c r="B5" s="7"/>
+      <c r="C5" s="7"/>
+      <c r="D5" s="7"/>
+      <c r="E5" s="7"/>
+      <c r="F5" s="7"/>
+      <c r="G5" s="7"/>
+      <c r="H5" s="7"/>
     </row>
     <row r="6" spans="1:8" ht="27" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="7" t="s">
+      <c r="A6" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="B6" s="10"/>
-      <c r="C6" s="10"/>
-      <c r="D6" s="10"/>
-      <c r="E6" s="10"/>
-      <c r="F6" s="10"/>
-      <c r="G6" s="10"/>
-      <c r="H6" s="10"/>
+      <c r="B6" s="9"/>
+      <c r="C6" s="9"/>
+      <c r="D6" s="9"/>
+      <c r="E6" s="9"/>
+      <c r="F6" s="9"/>
+      <c r="G6" s="9"/>
+      <c r="H6" s="9"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -2157,46 +2155,46 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="27" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="16" t="s">
+      <c r="A1" s="19" t="s">
         <v>83</v>
       </c>
-      <c r="B1" s="16"/>
+      <c r="B1" s="19"/>
     </row>
     <row r="2" spans="1:2" ht="27" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="7" t="s">
+      <c r="A2" s="6" t="s">
         <v>84</v>
       </c>
-      <c r="B2" s="8"/>
+      <c r="B2" s="7"/>
     </row>
     <row r="3" spans="1:2" ht="27" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="7" t="s">
+      <c r="A3" s="6" t="s">
         <v>79</v>
       </c>
-      <c r="B3" s="8"/>
+      <c r="B3" s="7"/>
     </row>
     <row r="4" spans="1:2" ht="27" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="7" t="s">
+      <c r="A4" s="6" t="s">
         <v>80</v>
       </c>
-      <c r="B4" s="8"/>
+      <c r="B4" s="7"/>
     </row>
     <row r="5" spans="1:2" ht="27" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="7" t="s">
+      <c r="A5" s="6" t="s">
         <v>81</v>
       </c>
-      <c r="B5" s="8"/>
+      <c r="B5" s="7"/>
     </row>
     <row r="6" spans="1:2" ht="27" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="7" t="s">
+      <c r="A6" s="6" t="s">
         <v>82</v>
       </c>
-      <c r="B6" s="8"/>
+      <c r="B6" s="7"/>
     </row>
     <row r="7" spans="1:2" ht="27" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="7" t="s">
+      <c r="A7" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="B7" s="8"/>
+      <c r="B7" s="7"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -2224,46 +2222,46 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="27" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="16" t="s">
+      <c r="A1" s="19" t="s">
         <v>85</v>
       </c>
-      <c r="B1" s="16"/>
+      <c r="B1" s="19"/>
     </row>
     <row r="2" spans="1:2" ht="27" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="9" t="s">
+      <c r="A2" s="8" t="s">
         <v>86</v>
       </c>
-      <c r="B2" s="8"/>
+      <c r="B2" s="7"/>
     </row>
     <row r="3" spans="1:2" ht="27" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="7" t="s">
+      <c r="A3" s="6" t="s">
         <v>84</v>
       </c>
-      <c r="B3" s="8"/>
+      <c r="B3" s="7"/>
     </row>
     <row r="4" spans="1:2" ht="27" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="7" t="s">
+      <c r="A4" s="6" t="s">
         <v>79</v>
       </c>
-      <c r="B4" s="8"/>
+      <c r="B4" s="7"/>
     </row>
     <row r="5" spans="1:2" ht="27" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="7" t="s">
+      <c r="A5" s="6" t="s">
         <v>80</v>
       </c>
-      <c r="B5" s="8"/>
+      <c r="B5" s="7"/>
     </row>
     <row r="6" spans="1:2" ht="27" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="7" t="s">
+      <c r="A6" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="B6" s="8"/>
+      <c r="B6" s="7"/>
     </row>
     <row r="7" spans="1:2" ht="27" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="7" t="s">
+      <c r="A7" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="B7" s="8"/>
+      <c r="B7" s="7"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>